<commit_message>
fix: NameError in method __init__
NameError: ERROR in method __init__ of class Conductor: kind object STR_SC does not exist.
Please check cell A1 in sheet <Worksheet "STACK"> of file conductor_1_input.xlsx.

modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_1_input.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_1_operation.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_3_HTS_HVDC/conductor_1_input.xlsx
+++ b/TDD_examples/CASE_3_HTS_HVDC/conductor_1_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_3_HTS_HVDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD64D15A-ECFC-46F5-9C72-F4BBDA470D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A33260-D0C7-4860-8F9D-4110B80C88E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="2" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>STR_SC</t>
-  </si>
-  <si>
     <t>row used to get the correct number of superconductor strands objects in cell B1 as the sum of values in this row starting from cell D2</t>
   </si>
   <si>
@@ -476,6 +473,9 @@
   </si>
   <si>
     <t>ge</t>
+  </si>
+  <si>
+    <t>STACK</t>
   </si>
 </sst>
 </file>
@@ -977,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
@@ -1086,7 +1086,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
@@ -1106,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -1132,7 +1132,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,7 +1159,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>13</v>
@@ -1168,7 +1168,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="14">
         <v>0</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>8</v>
@@ -1361,7 +1361,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" s="5" t="b">
         <v>0</v>
@@ -1381,11 +1381,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCDFC4-8F8B-44BE-BC94-0C08DE31F1F6}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:E26"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,7 +1400,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="B1" s="9">
         <f>SUM(E$2:EZ2)</f>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="7">
         <v>0</v>
@@ -1419,7 +1419,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="10">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="E3" s="9" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
-        <v>STR_SC_0</v>
+        <v>STACK_0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
@@ -1476,7 +1476,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="13">
         <v>0</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="6" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
@@ -1493,7 +1493,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="13">
         <v>0</v>
@@ -1518,16 +1518,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="E8" s="14">
         <v>1</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>13</v>
@@ -1544,13 +1544,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
@@ -1559,13 +1559,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>13</v>
@@ -1574,13 +1574,13 @@
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>13</v>
@@ -1589,13 +1589,13 @@
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>13</v>
@@ -1604,13 +1604,13 @@
         <v>5</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>13</v>
@@ -1619,28 +1619,28 @@
         <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
@@ -1649,13 +1649,13 @@
         <v>9</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>8</v>
@@ -1664,13 +1664,13 @@
         <v>9</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E17" s="14"/>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>8</v>
@@ -1679,13 +1679,13 @@
         <v>9</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>8</v>
@@ -1694,13 +1694,13 @@
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>8</v>
@@ -1709,7 +1709,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="14"/>
     </row>
@@ -1766,16 +1766,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="E24" s="5">
         <v>20</v>
@@ -1783,16 +1783,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="E25" s="5">
         <f>10^-5</f>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>8</v>
@@ -1810,14 +1810,14 @@
         <v>25</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="5" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1905,7 +1905,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
@@ -1922,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="13">
         <v>0</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
@@ -1939,7 +1939,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="13">
         <v>0</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
@@ -1973,7 +1973,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="14">
         <v>0</v>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -2024,7 +2024,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="16">
         <v>0</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>13</v>
@@ -2041,7 +2041,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>8</v>
@@ -2058,7 +2058,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13" s="13">
         <v>0</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>13</v>
@@ -2075,7 +2075,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E14" s="13">
         <v>0</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>8</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>8</v>
@@ -2143,7 +2143,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2193,35 +2193,35 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>8</v>
@@ -2230,7 +2230,7 @@
         <v>25</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2263,7 +2263,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="9">
         <f>SUM(E$2:Z2)</f>
@@ -2271,7 +2271,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2">
         <v>1</v>
@@ -2282,7 +2282,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="9">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
@@ -2340,7 +2340,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
@@ -2357,7 +2357,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>8</v>
@@ -2425,7 +2425,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="5" t="b">
         <v>0</v>
@@ -2462,7 +2462,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="9">
         <f>SUM(E$2:Z2)</f>
@@ -2470,7 +2470,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="7">
         <v>1</v>
@@ -2496,7 +2496,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="10">
         <f>IF(E$1 &gt; 0,1,0)</f>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -2576,7 +2576,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="13">
         <f>PI()/4*(0.024^2 - 0.02^2)</f>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>4</v>
@@ -2612,7 +2612,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="13">
         <v>0</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
@@ -2646,7 +2646,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="22">
         <v>0</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
@@ -2678,7 +2678,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="22">
         <v>0</v>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>13</v>
@@ -2710,7 +2710,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="13">
         <f>PI()*0.02</f>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>13</v>
@@ -2748,7 +2748,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="13">
         <f>PI()*0.024</f>
@@ -2786,7 +2786,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="15">
         <v>1</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -2818,30 +2818,30 @@
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
@@ -2850,25 +2850,25 @@
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>8</v>
@@ -2911,39 +2911,39 @@
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="F14" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="17" t="s">
+      <c r="J14" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E15" s="5">
         <v>0.8</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
@@ -2975,7 +2975,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="5" t="b">
         <v>0</v>

</xml_diff>